<commit_message>
fix: updated astra-v3 and added updated datasets
</commit_message>
<xml_diff>
--- a/models/astra-v3/training/dataset-clean-messages.xlsx
+++ b/models/astra-v3/training/dataset-clean-messages.xlsx
@@ -1,65 +1,56 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
-  <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
-  </bookViews>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <workbookPr/>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="39">
   <si>
-    <t xml:space="preserve">Tag</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Type (Injury or Treatment)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Meaning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Patterns</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Procedures</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Relations (Treatment or Procedures)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">References</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Context Set</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not related to First Aid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Message</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thank you for sharing! Just a note that this query isn’t directly related to first aid. Let me know if there's anything specific you’d like to discuss.
+    <t>Tag</t>
+  </si>
+  <si>
+    <t>Type (Injury or Treatment)</t>
+  </si>
+  <si>
+    <t>Meaning</t>
+  </si>
+  <si>
+    <t>Patterns</t>
+  </si>
+  <si>
+    <t>Procedures</t>
+  </si>
+  <si>
+    <t>Relations (Treatment or Procedures)</t>
+  </si>
+  <si>
+    <t>References</t>
+  </si>
+  <si>
+    <t>Context Set</t>
+  </si>
+  <si>
+    <t>Not related to first aid</t>
+  </si>
+  <si>
+    <t>Message</t>
+  </si>
+  <si>
+    <t>Thank you for sharing! Just a note that this query isn’t directly related to first aid. Let me know if there's anything specific you’d like to discuss.
 I appreciate your input! Please be advised that the query doesn't seem connected to first aid. If you need assistance on any other topic, just reach out.
 Thank you for your message! It appears this query isn’t related to first aid, but I’d be happy to help with any other questions you may have.
 Thank you for your inquiry! Kindly note that the query doesn't pertain to first aid. If you need help with any other topic, feel free to ask.
 Thanks for reaching out! This query seems unrelated to first aid. I’m here to help with anything else you might need, just let me know.</t>
   </si>
   <si>
-    <t xml:space="preserve">Where is the nearest library?
+    <t>Where is the nearest library?
 How to start a podcast?
 What are the top 10 tourist destinations in Japan?
 What is artificial intelligence?
@@ -203,17 +194,17 @@
 How to build an effective resume?</t>
   </si>
   <si>
-    <t xml:space="preserve">HIndi konektado sa First Aid</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Salamat po sa inyong pagbabahagi! Paalala lamang na ang query na ito ay hindi po direktang kaugnay ng first aid. Kung may partikular po kayong gustong pag-usapan, ipaalam lang po.
+    <t>Hindi konektado sa first aid</t>
+  </si>
+  <si>
+    <t>Salamat po sa inyong pagbabahagi! Paalala lamang na ang query na ito ay hindi po direktang kaugnay ng first aid. Kung may partikular po kayong gustong pag-usapan, ipaalam lang po.
 Maraming salamat po sa inyong input! Paumanhin po, ngunit ang query ay tila walang kaugnayan sa first aid. Kung may iba po kayong tanong, nandito lang po ako para tumulong.
 Salamat po sa inyong mensahe! Mukhang hindi po ito nauugnay sa first aid, ngunit masaya po akong tutulong kung may iba po kayong gustong itanong.
 Salamat po sa inyong pagtatanong! Tandaan lamang po na ang query ay hindi po konektado sa first aid. Kung kailangan niyo po ng tulong sa ibang bagay, ipagbigay-alam lang po.
 Salamat po sa inyong pag-abot! Mukhang hindi po konektado ang query na ito sa first aid. Nandito lang po ako kung may iba pa po kayong kailangan, ipaalam lang po.</t>
   </si>
   <si>
-    <t xml:space="preserve">Ano ang pinakamagandang paraan ng pagtitipid?
+    <t>Ano ang pinakamagandang paraan ng pagtitipid?
 Anong oras ang huling biyahe ng bus?
 Saan pwedeng bumili ng murang damit?
 Anong mga libreng online courses ang maganda?
@@ -265,15 +256,15 @@
 Saan pwedeng mag-enroll ng leadership course?</t>
   </si>
   <si>
-    <t xml:space="preserve">Not in Datasets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I apologize, but the query you submitted is not included in the dataset. Please let me know if there is anything else I can assist you with.
+    <t>Not in datasets</t>
+  </si>
+  <si>
+    <t>I apologize, but the query you submitted is not included in the dataset. Please let me know if there is anything else I can assist you with.
 Thank you for your inquiry! However, it seems that the information you are looking for is not present in the dataset. I'm here to help if you need further assistance.
 I appreciate your interest, but unfortunately, the query you provided is not available in the dataset. Please feel free to ask about other topics or queries!</t>
   </si>
   <si>
-    <t xml:space="preserve">Avulsions
+    <t>Avulsions
 Contusions
 Amputations
 Ribs
@@ -475,15 +466,15 @@
 Mission Statement</t>
   </si>
   <si>
-    <t xml:space="preserve">Wala sa Datasets</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paumanhin, ngunit ang katanungan na iyong isinumite ay hindi kasama sa dataset. Mangyaring ipaalam sa akin kung mayroon pa akong maitutulong sa iyo.
+    <t>Wala sa datasets</t>
+  </si>
+  <si>
+    <t>Paumanhin, ngunit ang katanungan na iyong isinumite ay hindi kasama sa dataset. Mangyaring ipaalam sa akin kung mayroon pa akong maitutulong sa iyo.
 Salamat sa iyong tanong! Subalit, mukhang hindi naroroon ang impormasyong hinahanap mo sa dataset. Nandito ako upang tumulong kung kailangan mo pa ng karagdagang tulong.
 Pinahahalagahan ko ang iyong interes, ngunit sa kasamaang palad, ang katanungan na iyong ibinigay ay wala sa dataset. Huwag mag-atubiling magtanong tungkol sa iba pang mga paksa o katanungan!</t>
   </si>
   <si>
-    <t xml:space="preserve">Pag-alis ng bahagi ng balat
+    <t>Pag-alis ng bahagi ng balat
 Kontusyon
 Amputasyon
 Bali ng mga Tadyang
@@ -632,10 +623,10 @@
 Mga Teknik sa Kam</t>
   </si>
   <si>
-    <t xml:space="preserve">greetings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hello! Thank you for visiting.
+    <t>Greetings</t>
+  </si>
+  <si>
+    <t>Hello! Thank you for visiting.
 How are you? I’m here to help you.
 Hi! How can I assist you today?
 Good day! How can I support you?
@@ -685,7 +676,7 @@
 Good day to all of you! If you have questions, I’m here to assist.</t>
   </si>
   <si>
-    <t xml:space="preserve">Hello!
+    <t>Hello!
 Hi there!
 How are you?
 Is anyone there?
@@ -734,10 +725,10 @@
 Good day to all of you!</t>
   </si>
   <si>
-    <t xml:space="preserve">Kamusta</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hello! Salamat sa pag-bisita.
+    <t>Kamusta</t>
+  </si>
+  <si>
+    <t>Hello! Salamat sa pag-bisita.
 Kamusta! Nandito ako para tumulong.
 Hi! Anong maitutulong ko sa iyo ngayon?
 Magandang araw! Paano kita matutulungan?
@@ -788,7 +779,7 @@
 Magandang araw sa iyong lahat! Kung may tanong, nandito ako para tumulong.</t>
   </si>
   <si>
-    <t xml:space="preserve">Hello!
+    <t>Hello!
 Kamusta!
 Hi!
 Magandang araw!
@@ -839,17 +830,17 @@
 Magandang araw sa iyong lahat!</t>
   </si>
   <si>
-    <t xml:space="preserve">Paalam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Paalam! Ingat ka at alagaan mo ang iyong sarili!
+    <t>Paalam</t>
+  </si>
+  <si>
+    <t>Paalam! Ingat ka at alagaan mo ang iyong sarili!
 Magandang araw! Tandaan, nandito ako kung kailangan mo ng payo sa first aid.
 Paalam! Huwag mag-atubiling bumalik kung may mga tanong ka pa tungkol sa first aid.
 Ingat! Nandito lang ako para tumulong tuwing kailangan mo ng tulong.
 Kita tayo muli! Mahalaga ang iyong kalusugan, at masaya akong makatulong!</t>
   </si>
   <si>
-    <t xml:space="preserve">Paalam sa ngayon
+    <t>Paalam sa ngayon
 Kitakits mamaya
 Ingat, paalam
 Hanggang sa susunod
@@ -871,17 +862,17 @@
 Magandang araw, paalam!</t>
   </si>
   <si>
-    <t xml:space="preserve">Goodbye</t>
-  </si>
-  <si>
-    <t xml:space="preserve">See you! Stay safe and take care of yourself!
+    <t>Goodbye</t>
+  </si>
+  <si>
+    <t>See you! Stay safe and take care of yourself!
 Have a nice day! Remember, I'm here if you need any first aid advice.
 Bye! Don’t hesitate to return if you have more questions about first aid.
 Take care! I'm always here to help whenever you need assistance.
 See you soon! Your health is important, and I'm glad to help!</t>
   </si>
   <si>
-    <t xml:space="preserve">Bye for now
+    <t>Bye for now
 Catch you later
 Take care, bye
 Until next time
@@ -903,10 +894,10 @@
 Have a great day, bye!</t>
   </si>
   <si>
-    <t xml:space="preserve">Thanks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I’m glad to assist!
+    <t>Thanks</t>
+  </si>
+  <si>
+    <t>I’m glad to assist!
 Always here to help!
 It’s my pleasure to support you!
 Happy to provide assistance!
@@ -918,7 +909,7 @@
 Your well-being is my priority!</t>
   </si>
   <si>
-    <t xml:space="preserve">Thank you so much
+    <t>Thank you so much
 I really appreciate it
 Thank you very much
 That’s incredibly helpful, thanks!
@@ -930,10 +921,10 @@
 Thanks a ton for everything!</t>
   </si>
   <si>
-    <t xml:space="preserve">Salamat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Masaya akong makatulong!
+    <t>Salamat</t>
+  </si>
+  <si>
+    <t>Masaya akong makatulong!
 Nandito lang ako para tumulong!
 Kasiyahan kong suportahan ka!
 Masaya akong magbigay ng tulong!
@@ -945,7 +936,7 @@
 Ang iyong kalusugan ang aking prayoridad!</t>
   </si>
   <si>
-    <t xml:space="preserve">Salamat nang marami
+    <t>Salamat nang marami
 Talagang pinahahalagahan ko ito
 Maraming salamat sa iyo
 Napakalaking tulong nito, salamat!
@@ -960,39 +951,18 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="2">
     <font>
-      <sz val="10"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
+      <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
-      <family val="0"/>
-      <charset val="1"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1000,66 +970,41 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+  <cellStyleXfs count="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+  </cellStyleXfs>
+  <cellXfs count="5">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-  </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+  <cellStyles count="1">
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1070,90 +1015,94 @@
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="000000"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4285f4"/>
+        <a:srgbClr val="4285F4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ea4335"/>
+        <a:srgbClr val="EA4335"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="fbbc04"/>
+        <a:srgbClr val="FBBC04"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="34a853"/>
+        <a:srgbClr val="34A853"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="ff6d01"/>
+        <a:srgbClr val="FF6D01"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="46bdc6"/>
+        <a:srgbClr val="46BDC6"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="1155cc"/>
+        <a:srgbClr val="1155CC"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="1155cc"/>
+        <a:srgbClr val="1155CC"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Sheets">
       <a:majorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:cs typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:ea typeface="Arial" pitchFamily="0" charset="1"/>
-        <a:cs typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Arial"/>
+        <a:ea typeface="Arial"/>
+        <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme>
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:gradFill>
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
                 <a:tint val="67000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
                 <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
                 <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
-        <a:gradFill>
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
                 <a:lumMod val="102000"/>
                 <a:tint val="94000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
                 <a:lumMod val="100000"/>
                 <a:shade val="100000"/>
               </a:schemeClr>
@@ -1161,24 +1110,33 @@
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
                 <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
         <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
@@ -1191,7 +1149,13 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
@@ -1201,13 +1165,15 @@
         <a:solidFill>
           <a:schemeClr val="phClr">
             <a:tint val="95000"/>
+            <a:satMod val="170000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:gradFill>
+        <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
                 <a:tint val="93000"/>
+                <a:satMod val="150000"/>
                 <a:shade val="98000"/>
                 <a:lumMod val="102000"/>
               </a:schemeClr>
@@ -1215,6 +1181,7 @@
             <a:gs pos="50000">
               <a:schemeClr val="phClr">
                 <a:tint val="98000"/>
+                <a:satMod val="130000"/>
                 <a:shade val="90000"/>
                 <a:lumMod val="103000"/>
               </a:schemeClr>
@@ -1222,11 +1189,11 @@
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
                 <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -1235,25 +1202,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J8" activeCellId="0" sqref="J8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="30.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.89"/>
+    <col customWidth="1" min="1" max="1" width="32.63"/>
+    <col customWidth="1" min="2" max="2" width="31.88"/>
+    <col customWidth="1" min="3" max="3" width="30.38"/>
+    <col customWidth="1" min="4" max="4" width="40.88"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1279,7 +1243,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -1293,29 +1257,29 @@
         <v>11</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
-      <c r="S2" s="2"/>
-      <c r="T2" s="2"/>
-      <c r="U2" s="2"/>
-      <c r="V2" s="2"/>
-      <c r="W2" s="2"/>
-      <c r="X2" s="2"/>
-      <c r="Y2" s="2"/>
-      <c r="Z2" s="2"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="3"/>
+      <c r="Z2" s="3"/>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3">
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
@@ -1328,30 +1292,30 @@
       <c r="D3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
-      <c r="S3" s="2"/>
-      <c r="T3" s="2"/>
-      <c r="U3" s="2"/>
-      <c r="V3" s="2"/>
-      <c r="W3" s="2"/>
-      <c r="X3" s="2"/>
-      <c r="Y3" s="2"/>
-      <c r="Z3" s="2"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+      <c r="V3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="X3" s="3"/>
+      <c r="Y3" s="3"/>
+      <c r="Z3" s="3"/>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4">
       <c r="A4" s="2" t="s">
         <v>15</v>
       </c>
@@ -1364,30 +1328,30 @@
       <c r="D4" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
-      <c r="S4" s="2"/>
-      <c r="T4" s="2"/>
-      <c r="U4" s="2"/>
-      <c r="V4" s="2"/>
-      <c r="W4" s="2"/>
-      <c r="X4" s="2"/>
-      <c r="Y4" s="2"/>
-      <c r="Z4" s="2"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="3"/>
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+      <c r="V4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="X4" s="3"/>
+      <c r="Y4" s="3"/>
+      <c r="Z4" s="3"/>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -1400,30 +1364,30 @@
       <c r="D5" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
-      <c r="S5" s="2"/>
-      <c r="T5" s="2"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="2"/>
-      <c r="W5" s="2"/>
-      <c r="X5" s="2"/>
-      <c r="Y5" s="2"/>
-      <c r="Z5" s="2"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="R5" s="3"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="U5" s="3"/>
+      <c r="V5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="3"/>
+      <c r="Z5" s="3"/>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6">
       <c r="A6" s="2" t="s">
         <v>21</v>
       </c>
@@ -1436,30 +1400,30 @@
       <c r="D6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="2"/>
-      <c r="W6" s="2"/>
-      <c r="X6" s="2"/>
-      <c r="Y6" s="2"/>
-      <c r="Z6" s="2"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="R6" s="3"/>
+      <c r="S6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="3"/>
+      <c r="V6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="X6" s="3"/>
+      <c r="Y6" s="3"/>
+      <c r="Z6" s="3"/>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
@@ -1472,30 +1436,30 @@
       <c r="D7" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="2"/>
-      <c r="W7" s="2"/>
-      <c r="X7" s="2"/>
-      <c r="Y7" s="2"/>
-      <c r="Z7" s="2"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="3"/>
+      <c r="S7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="U7" s="3"/>
+      <c r="V7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="X7" s="3"/>
+      <c r="Y7" s="3"/>
+      <c r="Z7" s="3"/>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8">
       <c r="A8" s="2" t="s">
         <v>27</v>
       </c>
@@ -1508,30 +1472,30 @@
       <c r="D8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="2"/>
-      <c r="R8" s="2"/>
-      <c r="S8" s="2"/>
-      <c r="T8" s="2"/>
-      <c r="U8" s="2"/>
-      <c r="V8" s="2"/>
-      <c r="W8" s="2"/>
-      <c r="X8" s="2"/>
-      <c r="Y8" s="2"/>
-      <c r="Z8" s="2"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+      <c r="M8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="R8" s="3"/>
+      <c r="S8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="U8" s="3"/>
+      <c r="V8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="X8" s="3"/>
+      <c r="Y8" s="3"/>
+      <c r="Z8" s="3"/>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9">
       <c r="A9" s="2" t="s">
         <v>30</v>
       </c>
@@ -1544,30 +1508,30 @@
       <c r="D9" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="2"/>
-      <c r="R9" s="2"/>
-      <c r="S9" s="2"/>
-      <c r="T9" s="2"/>
-      <c r="U9" s="2"/>
-      <c r="V9" s="2"/>
-      <c r="W9" s="2"/>
-      <c r="X9" s="2"/>
-      <c r="Y9" s="2"/>
-      <c r="Z9" s="2"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+      <c r="M9" s="3"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+      <c r="R9" s="3"/>
+      <c r="S9" s="3"/>
+      <c r="T9" s="3"/>
+      <c r="U9" s="3"/>
+      <c r="V9" s="3"/>
+      <c r="W9" s="3"/>
+      <c r="X9" s="3"/>
+      <c r="Y9" s="3"/>
+      <c r="Z9" s="3"/>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10">
       <c r="A10" s="2" t="s">
         <v>33</v>
       </c>
@@ -1580,30 +1544,30 @@
       <c r="D10" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="2"/>
-      <c r="O10" s="2"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="2"/>
-      <c r="R10" s="2"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="2"/>
-      <c r="U10" s="2"/>
-      <c r="V10" s="2"/>
-      <c r="W10" s="2"/>
-      <c r="X10" s="2"/>
-      <c r="Y10" s="2"/>
-      <c r="Z10" s="2"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="3"/>
+      <c r="S10" s="3"/>
+      <c r="T10" s="3"/>
+      <c r="U10" s="3"/>
+      <c r="V10" s="3"/>
+      <c r="W10" s="3"/>
+      <c r="X10" s="3"/>
+      <c r="Y10" s="3"/>
+      <c r="Z10" s="3"/>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11">
       <c r="A11" s="2" t="s">
         <v>36</v>
       </c>
@@ -1616,39 +1580,33 @@
       <c r="D11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2"/>
-      <c r="I11" s="2"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="2"/>
-      <c r="N11" s="2"/>
-      <c r="O11" s="2"/>
-      <c r="P11" s="2"/>
-      <c r="Q11" s="2"/>
-      <c r="R11" s="2"/>
-      <c r="S11" s="2"/>
-      <c r="T11" s="2"/>
-      <c r="U11" s="2"/>
-      <c r="V11" s="2"/>
-      <c r="W11" s="2"/>
-      <c r="X11" s="2"/>
-      <c r="Y11" s="2"/>
-      <c r="Z11" s="2"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="3"/>
+      <c r="S11" s="3"/>
+      <c r="T11" s="3"/>
+      <c r="U11" s="3"/>
+      <c r="V11" s="3"/>
+      <c r="W11" s="3"/>
+      <c r="X11" s="3"/>
+      <c r="Y11" s="3"/>
+      <c r="Z11" s="3"/>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="1"/>
+    <row r="12">
+      <c r="B12" s="4"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>